<commit_message>
2nd commit Changed the logic of datacompare for file compare testcase. Changed connections file for Db connection
</commit_message>
<xml_diff>
--- a/data/tables_queries.xlsx
+++ b/data/tables_queries.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Database_automation\Database_automation\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72D7B72-2C3B-481A-98C4-F135DA4641B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
@@ -82,16 +88,16 @@
     <t>,</t>
   </si>
   <si>
-    <t>G://Database_automation//files//client_data_target.csv</t>
-  </si>
-  <si>
-    <t>G://Database_automation//files//client_data_src.csv</t>
+    <t>D://Database_automation//Database_automation//files//client_data_src.csv</t>
+  </si>
+  <si>
+    <t>D://Database_automation//Database_automation//files//client_data_target.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,7 +186,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -188,6 +194,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -236,7 +245,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,9 +278,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -304,6 +330,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -479,25 +522,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="9" width="28.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" customWidth="1"/>
+    <col min="4" max="6" width="28.88671875" customWidth="1"/>
+    <col min="7" max="9" width="28.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -556,23 +599,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="8" width="28.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="5" width="28.88671875" customWidth="1"/>
+    <col min="6" max="8" width="28.109375" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -609,7 +652,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>20</v>
@@ -618,7 +661,7 @@
         <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>20</v>
@@ -634,24 +677,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding new code 05.04.2020
</commit_message>
<xml_diff>
--- a/data/tables_queries.xlsx
+++ b/data/tables_queries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Database_automation\Database_automation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72D7B72-2C3B-481A-98C4-F135DA4641B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344BB7C6-0CF3-4812-91A7-75E9DDC15C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>TC_No.</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>D://Database_automation//Database_automation//files//client_data_target.csv</t>
+  </si>
+  <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -526,7 +532,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,10 +606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,11 +617,11 @@
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="8" width="28.109375" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
+    <col min="6" max="9" width="28.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,10 +647,13 @@
         <v>14</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -668,6 +677,38 @@
       </c>
       <c r="H2" t="s">
         <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>